<commit_message>
AP V2 Code changes
</commit_message>
<xml_diff>
--- a/AP Digital Squarenine/AP V2 S9/Digital Mail to S9 - Dispatcher/Data/Config.xlsx
+++ b/AP Digital Squarenine/AP V2 S9/Digital Mail to S9 - Dispatcher/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NTMGRM.OOHPBTDIGS9\Documents\NA-Automation\Digital Mail to S9 - Dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NTMGRM.OOHPBTDIGS9\Documents\NA-Automation\DIgital S9_latest\ORC Folder RE\Digital Mail to S9 - Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FB9166-869D-45F1-B42D-AD36CACECC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A328E9-54AF-4294-A979-1C4F4762C34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -222,6 +222,15 @@
   </si>
   <si>
     <t>Digital_S9_PAID</t>
+  </si>
+  <si>
+    <t>Cloud_FolderPath</t>
+  </si>
+  <si>
+    <t>GMUSA_DigitalS9</t>
+  </si>
+  <si>
+    <t>GMUSA_FINANCE_AP_DigitalS9</t>
   </si>
 </sst>
 </file>
@@ -638,7 +647,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -802,7 +811,17 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -4003,15 +4022,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="7f25b792-b2ba-4b5c-8669-b39a27555406" xsi:nil="true"/>
@@ -4023,7 +4033,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010045A9A53AB2AD7C409EFC96CC55961B83" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="737d8429b8eb9892549b3c27dc155f66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="649a79cd-06e4-47a3-aac9-21cb806f3675" xmlns:ns3="7f25b792-b2ba-4b5c-8669-b39a27555406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3c35880a7ae30656a46222e88cc05a07" ns2:_="" ns3:_="">
     <xsd:import namespace="649a79cd-06e4-47a3-aac9-21cb806f3675"/>
@@ -4246,15 +4256,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C28C5D3-7254-4070-8A99-5DC238223FD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71F139BC-4B2F-41BD-9027-C55CC0C0F042}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4265,7 +4276,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FDDFF5D-6857-4772-8202-03097FC54C6B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4282,4 +4293,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C28C5D3-7254-4070-8A99-5DC238223FD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>